<commit_message>
Significantly upgraded the FactMiners MAGAZINE #GTS XML schema and generated a new set of issue metadata files. Also minor tweaks to a couple related data source files that will be migrated into the MAGAZINE format's publication metadata file.
Signed-off-by: Jim Salmons
</commit_message>
<xml_diff>
--- a/SoftalkTOCs_manifest.xlsx
+++ b/SoftalkTOCs_manifest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\OneDrive\GitHub\datasets_toc-masthead-adindex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salmo\OneDrive\GitHub\datasets_toc-masthead-adindex\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26085" windowHeight="12675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26087" windowHeight="12673"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="192">
   <si>
     <t>subject_id</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>ia_url</t>
+  </si>
+  <si>
+    <t>leafnum</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,6 +679,12 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -992,25 +1001,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2:E92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.41015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1024,19 +1034,22 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>190</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1049,21 +1062,24 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
         <v>29465</v>
       </c>
-      <c r="F2" t="str">
-        <f>("Softalk "&amp;" "&amp;TEXT(E2,"mmm-yyyy")&amp;" (V."&amp;C2&amp;" No."&amp;D2&amp;")")</f>
+      <c r="G2" t="str">
+        <f>("Softalk "&amp;" "&amp;TEXT(F2,"mmm-yyyy")&amp;" (V."&amp;C2&amp;" No."&amp;D2&amp;")")</f>
         <v>Softalk  Sep-1980 (V.1 No.1)</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1076,21 +1092,24 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3">
         <v>29495</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F91" si="0">("Softalk "&amp;" "&amp;TEXT(E3,"mmm-yyyy")&amp;" (V."&amp;C3&amp;" No."&amp;D3&amp;")")</f>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G91" si="0">("Softalk "&amp;" "&amp;TEXT(F3,"mmm-yyyy")&amp;" (V."&amp;C3&amp;" No."&amp;D3&amp;")")</f>
         <v>Softalk  Oct-1980 (V.1 No.2)</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1103,21 +1122,24 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
         <v>29526</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Nov-1980 (V.1 No.3)</v>
       </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
       <c r="H4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1130,21 +1152,24 @@
       <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="8">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3">
         <v>29526</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" ref="F5" si="1">("Softalk "&amp;" "&amp;TEXT(E5,"mmm-yyyy")&amp;" (V."&amp;C5&amp;" No."&amp;D5&amp;")")</f>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5" si="1">("Softalk "&amp;" "&amp;TEXT(F5,"mmm-yyyy")&amp;" (V."&amp;C5&amp;" No."&amp;D5&amp;")")</f>
         <v>Softalk  Nov-1980 (V.1 No.3)</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1157,21 +1182,24 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
         <v>29556</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Dec-1980 (V.1 No.4)</v>
       </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
       <c r="H6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1184,21 +1212,24 @@
       <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
         <v>29587</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jan-1981 (V.1 No.5)</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1211,21 +1242,24 @@
       <c r="D8" s="2">
         <v>6</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
         <v>29618</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Feb-1981 (V.1 No.6)</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1238,21 +1272,24 @@
       <c r="D9" s="2">
         <v>7</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
         <v>29646</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Mar-1981 (V.1 No.7)</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>7</v>
       </c>
-      <c r="H9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1265,21 +1302,24 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3">
         <v>29677</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Apr-1981 (V.1 No.8)</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1292,21 +1332,24 @@
       <c r="D11" s="2">
         <v>9</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3">
         <v>29707</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  May-1981 (V.1 No.9)</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1319,21 +1362,24 @@
       <c r="D12" s="2">
         <v>10</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="8">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
         <v>29738</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jun-1981 (V.1 No.10)</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1346,21 +1392,24 @@
       <c r="D13" s="2">
         <v>11</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
         <v>29768</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jul-1981 (V.1 No.11)</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1373,21 +1422,24 @@
       <c r="D14" s="2">
         <v>12</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="8">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
         <v>29799</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Aug-1981 (V.1 No.12)</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>12</v>
       </c>
-      <c r="H14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1400,21 +1452,24 @@
       <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6">
         <v>29830</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Sep-1981 (V.2 No.1)</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>13</v>
       </c>
-      <c r="H15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1427,21 +1482,24 @@
       <c r="D16" s="5">
         <v>2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="9">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6">
         <v>29860</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Oct-1981 (V.2 No.2)</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>14</v>
       </c>
-      <c r="H16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1454,21 +1512,24 @@
       <c r="D17" s="5">
         <v>3</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="9">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6">
         <v>29891</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Nov-1981 (V.2 No.3)</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>15</v>
       </c>
-      <c r="H17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1481,21 +1542,24 @@
       <c r="D18" s="5">
         <v>4</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="9">
+        <v>3</v>
+      </c>
+      <c r="F18" s="6">
         <v>29921</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Dec-1981 (V.2 No.4)</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1508,21 +1572,24 @@
       <c r="D19" s="5">
         <v>5</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="9">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6">
         <v>29952</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jan-1982 (V.2 No.5)</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>17</v>
       </c>
-      <c r="H19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1535,21 +1602,24 @@
       <c r="D20" s="5">
         <v>6</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="9">
+        <v>3</v>
+      </c>
+      <c r="F20" s="6">
         <v>29983</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Feb-1982 (V.2 No.6)</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>18</v>
       </c>
-      <c r="H20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1562,21 +1632,24 @@
       <c r="D21" s="5">
         <v>6</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="9">
+        <v>4</v>
+      </c>
+      <c r="F21" s="6">
         <v>29983</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" ref="F21" si="2">("Softalk "&amp;" "&amp;TEXT(E21,"mmm-yyyy")&amp;" (V."&amp;C21&amp;" No."&amp;D21&amp;")")</f>
+      <c r="G21" t="str">
+        <f t="shared" ref="G21" si="2">("Softalk "&amp;" "&amp;TEXT(F21,"mmm-yyyy")&amp;" (V."&amp;C21&amp;" No."&amp;D21&amp;")")</f>
         <v>Softalk  Feb-1982 (V.2 No.6)</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1589,21 +1662,24 @@
       <c r="D22" s="5">
         <v>7</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="9">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6">
         <v>30011</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Mar-1982 (V.2 No.7)</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>19</v>
       </c>
-      <c r="H22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1616,21 +1692,24 @@
       <c r="D23" s="5">
         <v>7</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="9">
+        <v>4</v>
+      </c>
+      <c r="F23" s="6">
         <v>30011</v>
       </c>
-      <c r="F23" t="str">
-        <f t="shared" ref="F23" si="3">("Softalk "&amp;" "&amp;TEXT(E23,"mmm-yyyy")&amp;" (V."&amp;C23&amp;" No."&amp;D23&amp;")")</f>
+      <c r="G23" t="str">
+        <f t="shared" ref="G23" si="3">("Softalk "&amp;" "&amp;TEXT(F23,"mmm-yyyy")&amp;" (V."&amp;C23&amp;" No."&amp;D23&amp;")")</f>
         <v>Softalk  Mar-1982 (V.2 No.7)</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="H23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1643,21 +1722,24 @@
       <c r="D24" s="5">
         <v>8</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="9">
+        <v>3</v>
+      </c>
+      <c r="F24" s="6">
         <v>30042</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Apr-1982 (V.2 No.8)</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>20</v>
       </c>
-      <c r="H24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1670,21 +1752,24 @@
       <c r="D25" s="5">
         <v>8</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="9">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6">
         <v>30042</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" ref="F25" si="4">("Softalk "&amp;" "&amp;TEXT(E25,"mmm-yyyy")&amp;" (V."&amp;C25&amp;" No."&amp;D25&amp;")")</f>
+      <c r="G25" t="str">
+        <f t="shared" ref="G25" si="4">("Softalk "&amp;" "&amp;TEXT(F25,"mmm-yyyy")&amp;" (V."&amp;C25&amp;" No."&amp;D25&amp;")")</f>
         <v>Softalk  Apr-1982 (V.2 No.8)</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1697,21 +1782,24 @@
       <c r="D26" s="5">
         <v>9</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="9">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6">
         <v>30072</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  May-1982 (V.2 No.9)</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>21</v>
       </c>
-      <c r="H26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1724,21 +1812,24 @@
       <c r="D27" s="5">
         <v>9</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="9">
+        <v>4</v>
+      </c>
+      <c r="F27" s="6">
         <v>30072</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" ref="F27" si="5">("Softalk "&amp;" "&amp;TEXT(E27,"mmm-yyyy")&amp;" (V."&amp;C27&amp;" No."&amp;D27&amp;")")</f>
+      <c r="G27" t="str">
+        <f t="shared" ref="G27" si="5">("Softalk "&amp;" "&amp;TEXT(F27,"mmm-yyyy")&amp;" (V."&amp;C27&amp;" No."&amp;D27&amp;")")</f>
         <v>Softalk  May-1982 (V.2 No.9)</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1751,21 +1842,24 @@
       <c r="D28" s="5">
         <v>10</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="9">
+        <v>3</v>
+      </c>
+      <c r="F28" s="6">
         <v>30103</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jun-1982 (V.2 No.10)</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>22</v>
       </c>
-      <c r="H28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1778,21 +1872,24 @@
       <c r="D29" s="5">
         <v>10</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="9">
+        <v>4</v>
+      </c>
+      <c r="F29" s="6">
         <v>30103</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" ref="F29" si="6">("Softalk "&amp;" "&amp;TEXT(E29,"mmm-yyyy")&amp;" (V."&amp;C29&amp;" No."&amp;D29&amp;")")</f>
+      <c r="G29" t="str">
+        <f t="shared" ref="G29" si="6">("Softalk "&amp;" "&amp;TEXT(F29,"mmm-yyyy")&amp;" (V."&amp;C29&amp;" No."&amp;D29&amp;")")</f>
         <v>Softalk  Jun-1982 (V.2 No.10)</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="H29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1805,21 +1902,24 @@
       <c r="D30" s="5">
         <v>11</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="9">
+        <v>3</v>
+      </c>
+      <c r="F30" s="6">
         <v>30133</v>
       </c>
-      <c r="F30" t="str">
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jul-1982 (V.2 No.11)</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>23</v>
       </c>
-      <c r="H30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1832,21 +1932,24 @@
       <c r="D31" s="5">
         <v>11</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="9">
+        <v>4</v>
+      </c>
+      <c r="F31" s="6">
         <v>30133</v>
       </c>
-      <c r="F31" t="str">
-        <f t="shared" ref="F31" si="7">("Softalk "&amp;" "&amp;TEXT(E31,"mmm-yyyy")&amp;" (V."&amp;C31&amp;" No."&amp;D31&amp;")")</f>
+      <c r="G31" t="str">
+        <f t="shared" ref="G31" si="7">("Softalk "&amp;" "&amp;TEXT(F31,"mmm-yyyy")&amp;" (V."&amp;C31&amp;" No."&amp;D31&amp;")")</f>
         <v>Softalk  Jul-1982 (V.2 No.11)</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="H31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1859,21 +1962,24 @@
       <c r="D32" s="5">
         <v>12</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="9">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6">
         <v>30164</v>
       </c>
-      <c r="F32" t="str">
+      <c r="G32" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Aug-1982 (V.2 No.12)</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>24</v>
       </c>
-      <c r="H32" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1886,21 +1992,24 @@
       <c r="D33" s="5">
         <v>12</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="9">
+        <v>4</v>
+      </c>
+      <c r="F33" s="6">
         <v>30164</v>
       </c>
-      <c r="F33" t="str">
-        <f t="shared" ref="F33" si="8">("Softalk "&amp;" "&amp;TEXT(E33,"mmm-yyyy")&amp;" (V."&amp;C33&amp;" No."&amp;D33&amp;")")</f>
+      <c r="G33" t="str">
+        <f t="shared" ref="G33" si="8">("Softalk "&amp;" "&amp;TEXT(F33,"mmm-yyyy")&amp;" (V."&amp;C33&amp;" No."&amp;D33&amp;")")</f>
         <v>Softalk  Aug-1982 (V.2 No.12)</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="H33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1913,21 +2022,24 @@
       <c r="D34" s="2">
         <v>1</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="8">
+        <v>3</v>
+      </c>
+      <c r="F34" s="3">
         <v>30195</v>
       </c>
-      <c r="F34" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Sep-1982 (V.3 No.1)</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>25</v>
       </c>
-      <c r="H34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1940,21 +2052,24 @@
       <c r="D35" s="2">
         <v>1</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="8">
+        <v>4</v>
+      </c>
+      <c r="F35" s="3">
         <v>30195</v>
       </c>
-      <c r="F35" t="str">
-        <f t="shared" ref="F35" si="9">("Softalk "&amp;" "&amp;TEXT(E35,"mmm-yyyy")&amp;" (V."&amp;C35&amp;" No."&amp;D35&amp;")")</f>
+      <c r="G35" t="str">
+        <f t="shared" ref="G35" si="9">("Softalk "&amp;" "&amp;TEXT(F35,"mmm-yyyy")&amp;" (V."&amp;C35&amp;" No."&amp;D35&amp;")")</f>
         <v>Softalk  Sep-1982 (V.3 No.1)</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="H35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1967,21 +2082,24 @@
       <c r="D36" s="2">
         <v>2</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="8">
+        <v>3</v>
+      </c>
+      <c r="F36" s="3">
         <v>30225</v>
       </c>
-      <c r="F36" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Oct-1982 (V.3 No.2)</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>26</v>
       </c>
-      <c r="H36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1994,21 +2112,24 @@
       <c r="D37" s="2">
         <v>2</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="8">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
         <v>30225</v>
       </c>
-      <c r="F37" t="str">
-        <f t="shared" ref="F37" si="10">("Softalk "&amp;" "&amp;TEXT(E37,"mmm-yyyy")&amp;" (V."&amp;C37&amp;" No."&amp;D37&amp;")")</f>
+      <c r="G37" t="str">
+        <f t="shared" ref="G37" si="10">("Softalk "&amp;" "&amp;TEXT(F37,"mmm-yyyy")&amp;" (V."&amp;C37&amp;" No."&amp;D37&amp;")")</f>
         <v>Softalk  Oct-1982 (V.3 No.2)</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2021,21 +2142,24 @@
       <c r="D38" s="2">
         <v>3</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="8">
+        <v>3</v>
+      </c>
+      <c r="F38" s="3">
         <v>30256</v>
       </c>
-      <c r="F38" t="str">
+      <c r="G38" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Nov-1982 (V.3 No.3)</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>27</v>
       </c>
-      <c r="H38" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2048,21 +2172,24 @@
       <c r="D39" s="2">
         <v>3</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="8">
+        <v>4</v>
+      </c>
+      <c r="F39" s="3">
         <v>30256</v>
       </c>
-      <c r="F39" t="str">
-        <f t="shared" ref="F39" si="11">("Softalk "&amp;" "&amp;TEXT(E39,"mmm-yyyy")&amp;" (V."&amp;C39&amp;" No."&amp;D39&amp;")")</f>
+      <c r="G39" t="str">
+        <f t="shared" ref="G39" si="11">("Softalk "&amp;" "&amp;TEXT(F39,"mmm-yyyy")&amp;" (V."&amp;C39&amp;" No."&amp;D39&amp;")")</f>
         <v>Softalk  Nov-1982 (V.3 No.3)</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H39" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2075,21 +2202,24 @@
       <c r="D40" s="2">
         <v>4</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="8">
+        <v>3</v>
+      </c>
+      <c r="F40" s="3">
         <v>30286</v>
       </c>
-      <c r="F40" t="str">
+      <c r="G40" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Dec-1982 (V.3 No.4)</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>28</v>
       </c>
-      <c r="H40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2102,21 +2232,24 @@
       <c r="D41" s="2">
         <v>4</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="8">
+        <v>4</v>
+      </c>
+      <c r="F41" s="3">
         <v>30286</v>
       </c>
-      <c r="F41" t="str">
-        <f t="shared" ref="F41" si="12">("Softalk "&amp;" "&amp;TEXT(E41,"mmm-yyyy")&amp;" (V."&amp;C41&amp;" No."&amp;D41&amp;")")</f>
+      <c r="G41" t="str">
+        <f t="shared" ref="G41" si="12">("Softalk "&amp;" "&amp;TEXT(F41,"mmm-yyyy")&amp;" (V."&amp;C41&amp;" No."&amp;D41&amp;")")</f>
         <v>Softalk  Dec-1982 (V.3 No.4)</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="H41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2129,21 +2262,24 @@
       <c r="D42" s="2">
         <v>5</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="8">
+        <v>3</v>
+      </c>
+      <c r="F42" s="3">
         <v>30317</v>
       </c>
-      <c r="F42" t="str">
+      <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jan-1983 (V.3 No.5)</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>29</v>
       </c>
-      <c r="H42" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2156,21 +2292,24 @@
       <c r="D43" s="2">
         <v>5</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="8">
+        <v>4</v>
+      </c>
+      <c r="F43" s="3">
         <v>30317</v>
       </c>
-      <c r="F43" t="str">
-        <f t="shared" ref="F43" si="13">("Softalk "&amp;" "&amp;TEXT(E43,"mmm-yyyy")&amp;" (V."&amp;C43&amp;" No."&amp;D43&amp;")")</f>
+      <c r="G43" t="str">
+        <f t="shared" ref="G43" si="13">("Softalk "&amp;" "&amp;TEXT(F43,"mmm-yyyy")&amp;" (V."&amp;C43&amp;" No."&amp;D43&amp;")")</f>
         <v>Softalk  Jan-1983 (V.3 No.5)</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="H43" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2183,21 +2322,24 @@
       <c r="D44" s="2">
         <v>6</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="8">
+        <v>3</v>
+      </c>
+      <c r="F44" s="3">
         <v>30348</v>
       </c>
-      <c r="F44" t="str">
+      <c r="G44" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Feb-1983 (V.3 No.6)</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>30</v>
       </c>
-      <c r="H44" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2210,21 +2352,24 @@
       <c r="D45" s="2">
         <v>6</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="8">
+        <v>4</v>
+      </c>
+      <c r="F45" s="3">
         <v>30348</v>
       </c>
-      <c r="F45" t="str">
-        <f t="shared" ref="F45" si="14">("Softalk "&amp;" "&amp;TEXT(E45,"mmm-yyyy")&amp;" (V."&amp;C45&amp;" No."&amp;D45&amp;")")</f>
+      <c r="G45" t="str">
+        <f t="shared" ref="G45" si="14">("Softalk "&amp;" "&amp;TEXT(F45,"mmm-yyyy")&amp;" (V."&amp;C45&amp;" No."&amp;D45&amp;")")</f>
         <v>Softalk  Feb-1983 (V.3 No.6)</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="H45" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="H45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2237,21 +2382,24 @@
       <c r="D46" s="2">
         <v>7</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="8">
+        <v>3</v>
+      </c>
+      <c r="F46" s="3">
         <v>30376</v>
       </c>
-      <c r="F46" t="str">
+      <c r="G46" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Mar-1983 (V.3 No.7)</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>31</v>
       </c>
-      <c r="H46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2264,21 +2412,24 @@
       <c r="D47" s="2">
         <v>7</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="8">
+        <v>4</v>
+      </c>
+      <c r="F47" s="3">
         <v>30376</v>
       </c>
-      <c r="F47" t="str">
-        <f t="shared" ref="F47" si="15">("Softalk "&amp;" "&amp;TEXT(E47,"mmm-yyyy")&amp;" (V."&amp;C47&amp;" No."&amp;D47&amp;")")</f>
+      <c r="G47" t="str">
+        <f t="shared" ref="G47" si="15">("Softalk "&amp;" "&amp;TEXT(F47,"mmm-yyyy")&amp;" (V."&amp;C47&amp;" No."&amp;D47&amp;")")</f>
         <v>Softalk  Mar-1983 (V.3 No.7)</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2291,21 +2442,24 @@
       <c r="D48" s="2">
         <v>8</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="8">
+        <v>3</v>
+      </c>
+      <c r="F48" s="3">
         <v>30407</v>
       </c>
-      <c r="F48" t="str">
+      <c r="G48" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Apr-1983 (V.3 No.8)</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>32</v>
       </c>
-      <c r="H48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2318,21 +2472,24 @@
       <c r="D49" s="2">
         <v>8</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="8">
+        <v>4</v>
+      </c>
+      <c r="F49" s="3">
         <v>30407</v>
       </c>
-      <c r="F49" t="str">
-        <f t="shared" ref="F49" si="16">("Softalk "&amp;" "&amp;TEXT(E49,"mmm-yyyy")&amp;" (V."&amp;C49&amp;" No."&amp;D49&amp;")")</f>
+      <c r="G49" t="str">
+        <f t="shared" ref="G49" si="16">("Softalk "&amp;" "&amp;TEXT(F49,"mmm-yyyy")&amp;" (V."&amp;C49&amp;" No."&amp;D49&amp;")")</f>
         <v>Softalk  Apr-1983 (V.3 No.8)</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="H49" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="H49" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2345,21 +2502,24 @@
       <c r="D50" s="2">
         <v>9</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="8">
+        <v>3</v>
+      </c>
+      <c r="F50" s="3">
         <v>30437</v>
       </c>
-      <c r="F50" t="str">
+      <c r="G50" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  May-1983 (V.3 No.9)</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>33</v>
       </c>
-      <c r="H50" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2372,21 +2532,24 @@
       <c r="D51" s="2">
         <v>9</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="8">
+        <v>4</v>
+      </c>
+      <c r="F51" s="3">
         <v>30437</v>
       </c>
-      <c r="F51" t="str">
-        <f t="shared" ref="F51" si="17">("Softalk "&amp;" "&amp;TEXT(E51,"mmm-yyyy")&amp;" (V."&amp;C51&amp;" No."&amp;D51&amp;")")</f>
+      <c r="G51" t="str">
+        <f t="shared" ref="G51" si="17">("Softalk "&amp;" "&amp;TEXT(F51,"mmm-yyyy")&amp;" (V."&amp;C51&amp;" No."&amp;D51&amp;")")</f>
         <v>Softalk  May-1983 (V.3 No.9)</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H51" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2399,21 +2562,24 @@
       <c r="D52" s="2">
         <v>10</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="8">
+        <v>3</v>
+      </c>
+      <c r="F52" s="3">
         <v>30468</v>
       </c>
-      <c r="F52" t="str">
+      <c r="G52" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jun-1983 (V.3 No.10)</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>34</v>
       </c>
-      <c r="H52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2426,21 +2592,24 @@
       <c r="D53" s="2">
         <v>10</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="8">
+        <v>4</v>
+      </c>
+      <c r="F53" s="3">
         <v>30468</v>
       </c>
-      <c r="F53" t="str">
-        <f t="shared" ref="F53" si="18">("Softalk "&amp;" "&amp;TEXT(E53,"mmm-yyyy")&amp;" (V."&amp;C53&amp;" No."&amp;D53&amp;")")</f>
+      <c r="G53" t="str">
+        <f t="shared" ref="G53" si="18">("Softalk "&amp;" "&amp;TEXT(F53,"mmm-yyyy")&amp;" (V."&amp;C53&amp;" No."&amp;D53&amp;")")</f>
         <v>Softalk  Jun-1983 (V.3 No.10)</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="H53" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="H53" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2453,21 +2622,24 @@
       <c r="D54" s="2">
         <v>11</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="8">
+        <v>3</v>
+      </c>
+      <c r="F54" s="3">
         <v>30498</v>
       </c>
-      <c r="F54" t="str">
+      <c r="G54" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jul-1983 (V.3 No.11)</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>35</v>
       </c>
-      <c r="H54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2480,21 +2652,24 @@
       <c r="D55" s="2">
         <v>11</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="8">
+        <v>4</v>
+      </c>
+      <c r="F55" s="3">
         <v>30498</v>
       </c>
-      <c r="F55" t="str">
-        <f t="shared" ref="F55" si="19">("Softalk "&amp;" "&amp;TEXT(E55,"mmm-yyyy")&amp;" (V."&amp;C55&amp;" No."&amp;D55&amp;")")</f>
+      <c r="G55" t="str">
+        <f t="shared" ref="G55" si="19">("Softalk "&amp;" "&amp;TEXT(F55,"mmm-yyyy")&amp;" (V."&amp;C55&amp;" No."&amp;D55&amp;")")</f>
         <v>Softalk  Jul-1983 (V.3 No.11)</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="H55" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="H55" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2507,21 +2682,24 @@
       <c r="D56" s="2">
         <v>12</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="8">
+        <v>3</v>
+      </c>
+      <c r="F56" s="3">
         <v>30529</v>
       </c>
-      <c r="F56" t="str">
+      <c r="G56" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Aug-1983 (V.3 No.12)</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>36</v>
       </c>
-      <c r="H56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2534,21 +2712,24 @@
       <c r="D57" s="2">
         <v>12</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="8">
+        <v>4</v>
+      </c>
+      <c r="F57" s="3">
         <v>30529</v>
       </c>
-      <c r="F57" t="str">
-        <f t="shared" ref="F57" si="20">("Softalk "&amp;" "&amp;TEXT(E57,"mmm-yyyy")&amp;" (V."&amp;C57&amp;" No."&amp;D57&amp;")")</f>
+      <c r="G57" t="str">
+        <f t="shared" ref="G57" si="20">("Softalk "&amp;" "&amp;TEXT(F57,"mmm-yyyy")&amp;" (V."&amp;C57&amp;" No."&amp;D57&amp;")")</f>
         <v>Softalk  Aug-1983 (V.3 No.12)</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H57" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2561,21 +2742,24 @@
       <c r="D58" s="5">
         <v>1</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="9">
+        <v>3</v>
+      </c>
+      <c r="F58" s="6">
         <v>30560</v>
       </c>
-      <c r="F58" t="str">
+      <c r="G58" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Sep-1983 (V.4 No.1)</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>37</v>
       </c>
-      <c r="H58" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2588,21 +2772,24 @@
       <c r="D59" s="5">
         <v>1</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="9">
+        <v>4</v>
+      </c>
+      <c r="F59" s="6">
         <v>30560</v>
       </c>
-      <c r="F59" t="str">
-        <f t="shared" ref="F59" si="21">("Softalk "&amp;" "&amp;TEXT(E59,"mmm-yyyy")&amp;" (V."&amp;C59&amp;" No."&amp;D59&amp;")")</f>
+      <c r="G59" t="str">
+        <f t="shared" ref="G59" si="21">("Softalk "&amp;" "&amp;TEXT(F59,"mmm-yyyy")&amp;" (V."&amp;C59&amp;" No."&amp;D59&amp;")")</f>
         <v>Softalk  Sep-1983 (V.4 No.1)</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="H59" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2615,21 +2802,24 @@
       <c r="D60" s="5">
         <v>2</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="9">
+        <v>4</v>
+      </c>
+      <c r="F60" s="6">
         <v>30590</v>
       </c>
-      <c r="F60" t="str">
+      <c r="G60" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Oct-1983 (V.4 No.2)</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>38</v>
       </c>
-      <c r="H60" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2642,21 +2832,24 @@
       <c r="D61" s="5">
         <v>2</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="9">
+        <v>5</v>
+      </c>
+      <c r="F61" s="6">
         <v>30590</v>
       </c>
-      <c r="F61" t="str">
+      <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Oct-1983 (V.4 No.2)</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>39</v>
       </c>
-      <c r="H61" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2669,21 +2862,24 @@
       <c r="D62" s="5">
         <v>2</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="9">
+        <v>6</v>
+      </c>
+      <c r="F62" s="6">
         <v>30590</v>
       </c>
-      <c r="F62" t="str">
-        <f t="shared" ref="F62" si="22">("Softalk "&amp;" "&amp;TEXT(E62,"mmm-yyyy")&amp;" (V."&amp;C62&amp;" No."&amp;D62&amp;")")</f>
+      <c r="G62" t="str">
+        <f t="shared" ref="G62" si="22">("Softalk "&amp;" "&amp;TEXT(F62,"mmm-yyyy")&amp;" (V."&amp;C62&amp;" No."&amp;D62&amp;")")</f>
         <v>Softalk  Oct-1983 (V.4 No.2)</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="H62" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2696,21 +2892,24 @@
       <c r="D63" s="5">
         <v>3</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="9">
+        <v>4</v>
+      </c>
+      <c r="F63" s="6">
         <v>30621</v>
       </c>
-      <c r="F63" t="str">
+      <c r="G63" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Nov-1983 (V.4 No.3)</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>40</v>
       </c>
-      <c r="H63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2723,21 +2922,24 @@
       <c r="D64" s="5">
         <v>3</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64" s="9">
+        <v>5</v>
+      </c>
+      <c r="F64" s="6">
         <v>30621</v>
       </c>
-      <c r="F64" t="str">
+      <c r="G64" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Nov-1983 (V.4 No.3)</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>41</v>
       </c>
-      <c r="H64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2750,21 +2952,24 @@
       <c r="D65" s="5">
         <v>3</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65" s="9">
+        <v>6</v>
+      </c>
+      <c r="F65" s="6">
         <v>30621</v>
       </c>
-      <c r="F65" t="str">
-        <f t="shared" ref="F65" si="23">("Softalk "&amp;" "&amp;TEXT(E65,"mmm-yyyy")&amp;" (V."&amp;C65&amp;" No."&amp;D65&amp;")")</f>
+      <c r="G65" t="str">
+        <f t="shared" ref="G65" si="23">("Softalk "&amp;" "&amp;TEXT(F65,"mmm-yyyy")&amp;" (V."&amp;C65&amp;" No."&amp;D65&amp;")")</f>
         <v>Softalk  Nov-1983 (V.4 No.3)</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="H65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2777,21 +2982,24 @@
       <c r="D66" s="5">
         <v>4</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E66" s="9">
+        <v>4</v>
+      </c>
+      <c r="F66" s="6">
         <v>30651</v>
       </c>
-      <c r="F66" t="str">
+      <c r="G66" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Dec-1983 (V.4 No.4)</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>42</v>
       </c>
-      <c r="H66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2804,21 +3012,24 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67" s="9">
+        <v>5</v>
+      </c>
+      <c r="F67" s="6">
         <v>30651</v>
       </c>
-      <c r="F67" t="str">
+      <c r="G67" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Dec-1983 (V.4 No.4)</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>43</v>
       </c>
-      <c r="H67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2831,21 +3042,24 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68" s="9">
+        <v>6</v>
+      </c>
+      <c r="F68" s="6">
         <v>30651</v>
       </c>
-      <c r="F68" t="str">
-        <f t="shared" ref="F68" si="24">("Softalk "&amp;" "&amp;TEXT(E68,"mmm-yyyy")&amp;" (V."&amp;C68&amp;" No."&amp;D68&amp;")")</f>
+      <c r="G68" t="str">
+        <f t="shared" ref="G68" si="24">("Softalk "&amp;" "&amp;TEXT(F68,"mmm-yyyy")&amp;" (V."&amp;C68&amp;" No."&amp;D68&amp;")")</f>
         <v>Softalk  Dec-1983 (V.4 No.4)</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="H68" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="H68" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2858,21 +3072,24 @@
       <c r="D69" s="5">
         <v>5</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69" s="9">
+        <v>4</v>
+      </c>
+      <c r="F69" s="6">
         <v>30682</v>
       </c>
-      <c r="F69" t="str">
+      <c r="G69" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jan-1984 (V.4 No.5)</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>44</v>
       </c>
-      <c r="H69" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2885,21 +3102,24 @@
       <c r="D70" s="5">
         <v>5</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="9">
+        <v>5</v>
+      </c>
+      <c r="F70" s="6">
         <v>30682</v>
       </c>
-      <c r="F70" t="str">
+      <c r="G70" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jan-1984 (V.4 No.5)</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>45</v>
       </c>
-      <c r="H70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2912,21 +3132,24 @@
       <c r="D71" s="5">
         <v>5</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71" s="9">
+        <v>6</v>
+      </c>
+      <c r="F71" s="6">
         <v>30682</v>
       </c>
-      <c r="F71" t="str">
-        <f t="shared" ref="F71" si="25">("Softalk "&amp;" "&amp;TEXT(E71,"mmm-yyyy")&amp;" (V."&amp;C71&amp;" No."&amp;D71&amp;")")</f>
+      <c r="G71" t="str">
+        <f t="shared" ref="G71" si="25">("Softalk "&amp;" "&amp;TEXT(F71,"mmm-yyyy")&amp;" (V."&amp;C71&amp;" No."&amp;D71&amp;")")</f>
         <v>Softalk  Jan-1984 (V.4 No.5)</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H71" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2939,21 +3162,24 @@
       <c r="D72" s="5">
         <v>6</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72" s="9">
+        <v>4</v>
+      </c>
+      <c r="F72" s="6">
         <v>30713</v>
       </c>
-      <c r="F72" t="str">
+      <c r="G72" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Feb-1984 (V.4 No.6)</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>46</v>
       </c>
-      <c r="H72" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2966,21 +3192,24 @@
       <c r="D73" s="5">
         <v>6</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="9">
+        <v>5</v>
+      </c>
+      <c r="F73" s="6">
         <v>30713</v>
       </c>
-      <c r="F73" t="str">
+      <c r="G73" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Feb-1984 (V.4 No.6)</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>47</v>
       </c>
-      <c r="H73" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2993,21 +3222,24 @@
       <c r="D74" s="5">
         <v>6</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74" s="9">
+        <v>6</v>
+      </c>
+      <c r="F74" s="6">
         <v>30713</v>
       </c>
-      <c r="F74" t="str">
-        <f t="shared" ref="F74" si="26">("Softalk "&amp;" "&amp;TEXT(E74,"mmm-yyyy")&amp;" (V."&amp;C74&amp;" No."&amp;D74&amp;")")</f>
+      <c r="G74" t="str">
+        <f t="shared" ref="G74" si="26">("Softalk "&amp;" "&amp;TEXT(F74,"mmm-yyyy")&amp;" (V."&amp;C74&amp;" No."&amp;D74&amp;")")</f>
         <v>Softalk  Feb-1984 (V.4 No.6)</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="H74" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="H74" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3020,21 +3252,24 @@
       <c r="D75" s="5">
         <v>7</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75" s="9">
+        <v>4</v>
+      </c>
+      <c r="F75" s="6">
         <v>30742</v>
       </c>
-      <c r="F75" t="str">
+      <c r="G75" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Mar-1984 (V.4 No.7)</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>48</v>
       </c>
-      <c r="H75" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3047,21 +3282,24 @@
       <c r="D76" s="5">
         <v>7</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="9">
+        <v>5</v>
+      </c>
+      <c r="F76" s="6">
         <v>30742</v>
       </c>
-      <c r="F76" t="str">
+      <c r="G76" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Mar-1984 (V.4 No.7)</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>49</v>
       </c>
-      <c r="H76" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3074,21 +3312,24 @@
       <c r="D77" s="5">
         <v>7</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77" s="9">
+        <v>6</v>
+      </c>
+      <c r="F77" s="6">
         <v>30742</v>
       </c>
-      <c r="F77" t="str">
-        <f t="shared" ref="F77" si="27">("Softalk "&amp;" "&amp;TEXT(E77,"mmm-yyyy")&amp;" (V."&amp;C77&amp;" No."&amp;D77&amp;")")</f>
+      <c r="G77" t="str">
+        <f t="shared" ref="G77" si="27">("Softalk "&amp;" "&amp;TEXT(F77,"mmm-yyyy")&amp;" (V."&amp;C77&amp;" No."&amp;D77&amp;")")</f>
         <v>Softalk  Mar-1984 (V.4 No.7)</v>
       </c>
-      <c r="G77" s="7" t="s">
+      <c r="H77" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="H77" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3101,21 +3342,24 @@
       <c r="D78" s="5">
         <v>8</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="9">
+        <v>4</v>
+      </c>
+      <c r="F78" s="6">
         <v>30773</v>
       </c>
-      <c r="F78" t="str">
+      <c r="G78" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Apr-1984 (V.4 No.8)</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>50</v>
       </c>
-      <c r="H78" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3128,21 +3372,24 @@
       <c r="D79" s="5">
         <v>8</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="9">
+        <v>5</v>
+      </c>
+      <c r="F79" s="6">
         <v>30773</v>
       </c>
-      <c r="F79" t="str">
+      <c r="G79" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Apr-1984 (V.4 No.8)</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>51</v>
       </c>
-      <c r="H79" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3155,21 +3402,24 @@
       <c r="D80" s="5">
         <v>8</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="9">
+        <v>6</v>
+      </c>
+      <c r="F80" s="6">
         <v>30773</v>
       </c>
-      <c r="F80" t="str">
-        <f t="shared" ref="F80" si="28">("Softalk "&amp;" "&amp;TEXT(E80,"mmm-yyyy")&amp;" (V."&amp;C80&amp;" No."&amp;D80&amp;")")</f>
+      <c r="G80" t="str">
+        <f t="shared" ref="G80" si="28">("Softalk "&amp;" "&amp;TEXT(F80,"mmm-yyyy")&amp;" (V."&amp;C80&amp;" No."&amp;D80&amp;")")</f>
         <v>Softalk  Apr-1984 (V.4 No.8)</v>
       </c>
-      <c r="G80" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="H80" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3182,21 +3432,24 @@
       <c r="D81" s="5">
         <v>9</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="9">
+        <v>4</v>
+      </c>
+      <c r="F81" s="6">
         <v>30803</v>
       </c>
-      <c r="F81" t="str">
+      <c r="G81" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  May-1984 (V.4 No.9)</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>52</v>
       </c>
-      <c r="H81" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3209,21 +3462,24 @@
       <c r="D82" s="5">
         <v>9</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="9">
+        <v>5</v>
+      </c>
+      <c r="F82" s="6">
         <v>30803</v>
       </c>
-      <c r="F82" t="str">
+      <c r="G82" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  May-1984 (V.4 No.9)</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>53</v>
       </c>
-      <c r="H82" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3236,21 +3492,24 @@
       <c r="D83" s="5">
         <v>9</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="9">
+        <v>6</v>
+      </c>
+      <c r="F83" s="6">
         <v>30803</v>
       </c>
-      <c r="F83" t="str">
-        <f t="shared" ref="F83" si="29">("Softalk "&amp;" "&amp;TEXT(E83,"mmm-yyyy")&amp;" (V."&amp;C83&amp;" No."&amp;D83&amp;")")</f>
+      <c r="G83" t="str">
+        <f t="shared" ref="G83" si="29">("Softalk "&amp;" "&amp;TEXT(F83,"mmm-yyyy")&amp;" (V."&amp;C83&amp;" No."&amp;D83&amp;")")</f>
         <v>Softalk  May-1984 (V.4 No.9)</v>
       </c>
-      <c r="G83" s="7" t="s">
+      <c r="H83" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="H83" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3263,21 +3522,24 @@
       <c r="D84" s="5">
         <v>10</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="9">
+        <v>4</v>
+      </c>
+      <c r="F84" s="6">
         <v>30834</v>
       </c>
-      <c r="F84" t="str">
+      <c r="G84" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jun-1984 (V.4 No.10)</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>54</v>
       </c>
-      <c r="H84" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3290,21 +3552,24 @@
       <c r="D85" s="5">
         <v>10</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="9">
+        <v>5</v>
+      </c>
+      <c r="F85" s="6">
         <v>30834</v>
       </c>
-      <c r="F85" t="str">
+      <c r="G85" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jun-1984 (V.4 No.10)</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>55</v>
       </c>
-      <c r="H85" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3317,21 +3582,24 @@
       <c r="D86" s="5">
         <v>10</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86" s="9">
+        <v>6</v>
+      </c>
+      <c r="F86" s="6">
         <v>30834</v>
       </c>
-      <c r="F86" t="str">
-        <f t="shared" ref="F86" si="30">("Softalk "&amp;" "&amp;TEXT(E86,"mmm-yyyy")&amp;" (V."&amp;C86&amp;" No."&amp;D86&amp;")")</f>
+      <c r="G86" t="str">
+        <f t="shared" ref="G86" si="30">("Softalk "&amp;" "&amp;TEXT(F86,"mmm-yyyy")&amp;" (V."&amp;C86&amp;" No."&amp;D86&amp;")")</f>
         <v>Softalk  Jun-1984 (V.4 No.10)</v>
       </c>
-      <c r="G86" s="7" t="s">
+      <c r="H86" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="H86" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3344,21 +3612,24 @@
       <c r="D87" s="5">
         <v>11</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87" s="9">
+        <v>4</v>
+      </c>
+      <c r="F87" s="6">
         <v>30864</v>
       </c>
-      <c r="F87" t="str">
+      <c r="G87" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jul-1984 (V.4 No.11)</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>56</v>
       </c>
-      <c r="H87" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3371,21 +3642,24 @@
       <c r="D88" s="5">
         <v>11</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E88" s="9">
+        <v>5</v>
+      </c>
+      <c r="F88" s="6">
         <v>30864</v>
       </c>
-      <c r="F88" t="str">
+      <c r="G88" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Jul-1984 (V.4 No.11)</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>57</v>
       </c>
-      <c r="H88" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3398,21 +3672,24 @@
       <c r="D89" s="5">
         <v>11</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E89" s="9">
+        <v>6</v>
+      </c>
+      <c r="F89" s="6">
         <v>30864</v>
       </c>
-      <c r="F89" t="str">
-        <f t="shared" ref="F89" si="31">("Softalk "&amp;" "&amp;TEXT(E89,"mmm-yyyy")&amp;" (V."&amp;C89&amp;" No."&amp;D89&amp;")")</f>
+      <c r="G89" t="str">
+        <f t="shared" ref="G89" si="31">("Softalk "&amp;" "&amp;TEXT(F89,"mmm-yyyy")&amp;" (V."&amp;C89&amp;" No."&amp;D89&amp;")")</f>
         <v>Softalk  Jul-1984 (V.4 No.11)</v>
       </c>
-      <c r="G89" s="7" t="s">
+      <c r="H89" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="H89" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3425,21 +3702,24 @@
       <c r="D90" s="5">
         <v>12</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="9">
+        <v>4</v>
+      </c>
+      <c r="F90" s="6">
         <v>30895</v>
       </c>
-      <c r="F90" t="str">
+      <c r="G90" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Aug-1984 (V.4 No.12)</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>58</v>
       </c>
-      <c r="H90" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3452,21 +3732,24 @@
       <c r="D91" s="5">
         <v>12</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="9">
+        <v>5</v>
+      </c>
+      <c r="F91" s="6">
         <v>30895</v>
       </c>
-      <c r="F91" t="str">
+      <c r="G91" t="str">
         <f t="shared" si="0"/>
         <v>Softalk  Aug-1984 (V.4 No.12)</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>59</v>
       </c>
-      <c r="H91" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3479,55 +3762,58 @@
       <c r="D92" s="5">
         <v>12</v>
       </c>
-      <c r="E92" s="6">
+      <c r="E92" s="9">
+        <v>6</v>
+      </c>
+      <c r="F92" s="6">
         <v>30895</v>
       </c>
-      <c r="F92" t="str">
-        <f t="shared" ref="F92" si="32">("Softalk "&amp;" "&amp;TEXT(E92,"mmm-yyyy")&amp;" (V."&amp;C92&amp;" No."&amp;D92&amp;")")</f>
+      <c r="G92" t="str">
+        <f t="shared" ref="G92" si="32">("Softalk "&amp;" "&amp;TEXT(F92,"mmm-yyyy")&amp;" (V."&amp;C92&amp;" No."&amp;D92&amp;")")</f>
         <v>Softalk  Aug-1984 (V.4 No.12)</v>
       </c>
-      <c r="G92" s="7" t="s">
+      <c r="H92" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G21" r:id="rId3"/>
-    <hyperlink ref="G23" r:id="rId4"/>
-    <hyperlink ref="G25" r:id="rId5"/>
-    <hyperlink ref="G27" r:id="rId6"/>
-    <hyperlink ref="G29" r:id="rId7"/>
-    <hyperlink ref="G31" r:id="rId8"/>
-    <hyperlink ref="G33" r:id="rId9"/>
-    <hyperlink ref="G35" r:id="rId10"/>
-    <hyperlink ref="G37" r:id="rId11"/>
-    <hyperlink ref="G39" r:id="rId12"/>
-    <hyperlink ref="G41" r:id="rId13"/>
-    <hyperlink ref="G43" r:id="rId14"/>
-    <hyperlink ref="G45" r:id="rId15"/>
-    <hyperlink ref="G47" r:id="rId16"/>
-    <hyperlink ref="G49" r:id="rId17"/>
-    <hyperlink ref="G51" r:id="rId18"/>
-    <hyperlink ref="G53" r:id="rId19"/>
-    <hyperlink ref="G55" r:id="rId20"/>
-    <hyperlink ref="G57" r:id="rId21"/>
-    <hyperlink ref="G59" r:id="rId22"/>
-    <hyperlink ref="G62" r:id="rId23"/>
-    <hyperlink ref="G65" r:id="rId24"/>
-    <hyperlink ref="G68" r:id="rId25"/>
-    <hyperlink ref="G71" r:id="rId26"/>
-    <hyperlink ref="G74" r:id="rId27"/>
-    <hyperlink ref="G77" r:id="rId28"/>
-    <hyperlink ref="G80" r:id="rId29"/>
-    <hyperlink ref="G83" r:id="rId30"/>
-    <hyperlink ref="G86" r:id="rId31"/>
-    <hyperlink ref="G89" r:id="rId32"/>
-    <hyperlink ref="G92" r:id="rId33"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="H21" r:id="rId3"/>
+    <hyperlink ref="H23" r:id="rId4"/>
+    <hyperlink ref="H25" r:id="rId5"/>
+    <hyperlink ref="H27" r:id="rId6"/>
+    <hyperlink ref="H29" r:id="rId7"/>
+    <hyperlink ref="H31" r:id="rId8"/>
+    <hyperlink ref="H33" r:id="rId9"/>
+    <hyperlink ref="H35" r:id="rId10"/>
+    <hyperlink ref="H37" r:id="rId11"/>
+    <hyperlink ref="H39" r:id="rId12"/>
+    <hyperlink ref="H41" r:id="rId13"/>
+    <hyperlink ref="H43" r:id="rId14"/>
+    <hyperlink ref="H45" r:id="rId15"/>
+    <hyperlink ref="H47" r:id="rId16"/>
+    <hyperlink ref="H49" r:id="rId17"/>
+    <hyperlink ref="H51" r:id="rId18"/>
+    <hyperlink ref="H53" r:id="rId19"/>
+    <hyperlink ref="H55" r:id="rId20"/>
+    <hyperlink ref="H57" r:id="rId21"/>
+    <hyperlink ref="H59" r:id="rId22"/>
+    <hyperlink ref="H62" r:id="rId23"/>
+    <hyperlink ref="H65" r:id="rId24"/>
+    <hyperlink ref="H68" r:id="rId25"/>
+    <hyperlink ref="H71" r:id="rId26"/>
+    <hyperlink ref="H74" r:id="rId27"/>
+    <hyperlink ref="H77" r:id="rId28"/>
+    <hyperlink ref="H80" r:id="rId29"/>
+    <hyperlink ref="H83" r:id="rId30"/>
+    <hyperlink ref="H86" r:id="rId31"/>
+    <hyperlink ref="H89" r:id="rId32"/>
+    <hyperlink ref="H92" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId34"/>

</xml_diff>